<commit_message>
rename function name and rewrite the function
</commit_message>
<xml_diff>
--- a/data/Case.xlsx
+++ b/data/Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenxi/PycharmProjects/gx-interface/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45E00BFB-87F7-DA4E-AC8F-C120D0257C7C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39ECFAD4-DC4E-364C-B26E-04AE5F9071B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="15800" xr2:uid="{8B2DD1EF-A30E-DB49-B0E0-60079CBD05CC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -56,6 +56,26 @@
   </si>
   <si>
     <t>except</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://192.168.1.86:80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/qc-engine/v3/sysusers/login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>POST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"userName": "admin", "password": "123"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>msg</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -63,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -74,6 +94,15 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
@@ -97,18 +126,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -420,15 +456,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6A1AFA-96C0-674C-9A2C-1BD4205C3AE7}">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,10 +491,39 @@
       </c>
       <c r="H1" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>200</v>
+      </c>
+      <c r="H2">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{167E5A34-14FA-464B-969B-B8E513DCD544}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>